<commit_message>
smv tg: update fed figures (change s to m)
</commit_message>
<xml_diff>
--- a/smv/figures/fed_calc.xlsx
+++ b/smv/figures/fed_calc.xlsx
@@ -1,17 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gforney\FireModels_fork\fig\smv\figures\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEEF64B-D15B-4BCF-975F-1DBD9005C97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="22035" windowHeight="11820"/>
+    <workbookView xWindow="768" yWindow="1920" windowWidth="29952" windowHeight="16104" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -57,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,12 +118,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -337,9 +359,13 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-30CC-4BA9-8105-D9BED27C141D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -368,12 +394,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>t (s)</a:t>
+                  <a:t>t (m)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -408,7 +433,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -449,7 +473,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -510,7 +540,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -543,9 +573,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -578,6 +625,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -753,16 +817,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -773,7 +837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -784,7 +848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>10000</v>
       </c>
@@ -795,12 +859,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>3.9100000000000003E-2</v>
@@ -809,7 +873,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -823,7 +887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -840,7 +904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -861,7 +925,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>A7+0.5</f>
         <v>0.5</v>
@@ -883,29 +947,29 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" ref="A9:A31" si="0">A8+0.5</f>
+        <f t="shared" ref="A9:A27" si="0">A8+0.5</f>
         <v>1</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B41" si="1">C9*E9+D9</f>
+        <f t="shared" ref="B9:B27" si="1">C9*E9+D9</f>
         <v>1.144215703298153</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C41" si="2">2.764*$B$3^1.036*A9/100000</f>
+        <f t="shared" ref="C9:C27" si="2">2.764*$B$3^1.036*A9/100000</f>
         <v>0.385068540334082</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D41" si="3">EXP(-8.13+0.54*(20.9-$D$3))*A9</f>
+        <f t="shared" ref="D9:D27" si="3">EXP(-8.13+0.54*(20.9-$D$3))*A9</f>
         <v>0.10603352089534795</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E41" si="4">EXP(0.1903*$C$3+2.0004)/7.1</f>
-        <v>2.6960971194948504</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E9:E37" si="4">EXP(0.1903*$C$3+2.0004)/7.1</f>
+        <v>2.6960971194948504</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1.5</v>
@@ -927,7 +991,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -949,7 +1013,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>2.5</v>
@@ -971,7 +1035,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -993,7 +1057,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>3.5</v>
@@ -1015,7 +1079,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1037,7 +1101,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>4.5</v>
@@ -1059,7 +1123,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1081,7 +1145,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>5.5</v>
@@ -1103,7 +1167,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1125,7 +1189,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>6.5</v>
@@ -1147,7 +1211,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1169,7 +1233,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>7.5</v>
@@ -1191,7 +1255,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1213,7 +1277,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>8.5</v>
@@ -1235,7 +1299,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1257,7 +1321,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>9.5</v>
@@ -1279,7 +1343,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1301,7 +1365,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" ref="A28:A37" si="5">A27+0.5</f>
         <v>10.5</v>
@@ -1323,7 +1387,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="5"/>
         <v>11</v>
@@ -1345,7 +1409,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="5"/>
         <v>11.5</v>
@@ -1367,7 +1431,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="5"/>
         <v>12</v>
@@ -1389,7 +1453,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="5"/>
         <v>12.5</v>
@@ -1411,7 +1475,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="5"/>
         <v>13</v>
@@ -1433,7 +1497,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="5"/>
         <v>13.5</v>
@@ -1455,7 +1519,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="5"/>
         <v>14</v>
@@ -1477,7 +1541,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="5"/>
         <v>14.5</v>
@@ -1499,7 +1563,7 @@
         <v>2.6960971194948504</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="5"/>
         <v>15</v>
@@ -1529,24 +1593,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>